<commit_message>
Finalizamos la reserva matemática
</commit_message>
<xml_diff>
--- a/TABLAS_DE_MORTALIDAD_1998-2003.xlsx
+++ b/TABLAS_DE_MORTALIDAD_1998-2003.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7973f5c145c6be4/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRA\PRA_Reservas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{4487D8A6-D1AD-4C1B-8255-5DDE8F936743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{750C43A2-DCFC-448A-840B-1393F6B4EE50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA8DEC9-4637-4258-8062-DCE38B101BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E51036F9-78CF-482E-AB75-CBE0FABE9E01}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="22275" windowHeight="8595" xr2:uid="{E51036F9-78CF-482E-AB75-CBE0FABE9E01}"/>
   </bookViews>
   <sheets>
     <sheet name="Hombres" sheetId="1" r:id="rId1"/>
     <sheet name="Mujeres" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,16 +42,16 @@
     <t>x</t>
   </si>
   <si>
-    <t>l(x)</t>
+    <t>ex</t>
   </si>
   <si>
-    <t>d(x)</t>
+    <t>lx</t>
   </si>
   <si>
-    <t>q(x)</t>
+    <t>dx</t>
   </si>
   <si>
-    <t>e^0 (x)</t>
+    <t>qx</t>
   </si>
 </sst>
 </file>
@@ -476,7 +475,7 @@
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,16 +491,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2053,7 +2052,7 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,16 +2066,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>